<commit_message>
Updated the cucumber feature file
</commit_message>
<xml_diff>
--- a/src/main/resources/ClearTrip1.xlsx
+++ b/src/main/resources/ClearTrip1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Surbhi_Modi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Surbhi_Modi\Downloads\cucumberSeleniumFramework-master\TestClearTrip\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F245DF-D47F-4FBE-B7A3-517A4B8EC96A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2BD51D-9299-402E-94DB-47A7970A90B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" xr2:uid="{2BF457D8-A8C4-43C2-A35B-4A2A2E4FE754}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>TripType</t>
   </si>
@@ -82,6 +82,27 @@
   </si>
   <si>
     <t>From</t>
+  </si>
+  <si>
+    <t>From1</t>
+  </si>
+  <si>
+    <t>To1</t>
+  </si>
+  <si>
+    <t>From2</t>
+  </si>
+  <si>
+    <t>To2</t>
+  </si>
+  <si>
+    <t>From3</t>
+  </si>
+  <si>
+    <t>To3</t>
+  </si>
+  <si>
+    <t>Pune</t>
   </si>
 </sst>
 </file>
@@ -433,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA7D650-469B-4986-9137-01419931BE43}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +469,7 @@
     <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,8 +500,26 @@
       <c r="J1" t="s">
         <v>12</v>
       </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -512,7 +551,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -544,7 +583,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -574,6 +613,24 @@
       </c>
       <c r="J4" t="s">
         <v>14</v>
+      </c>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>